<commit_message>
fixed display of value when swipping back
</commit_message>
<xml_diff>
--- a/extras/example-form/Example form - slider.xlsx
+++ b/extras/example-form/Example form - slider.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cking/github/surveycto-field-plug-ins/slider/extras/example-form/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitow\Documents\SurveyCTO Plugins\sliders\extras\example-form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADA0853-FD42-4948-8D8D-946CA3E48165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5A1088-4474-41F1-8146-42FB8150A936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44640" yWindow="8680" windowWidth="30120" windowHeight="20240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="384">
   <si>
     <t>type</t>
   </si>
@@ -3001,9 +3003,6 @@
   </si>
   <si>
     <t>custom-slider(min="0",max="100", step=1)</t>
-  </si>
-  <si>
-    <t>Slider Range 0 - 20</t>
   </si>
   <si>
     <t>Slider Range 0 - 1</t>
@@ -3022,7 +3021,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mmm"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -5460,40 +5459,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK17"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="29" style="1" customWidth="1"/>
     <col min="2" max="2" width="40.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="30.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="23" style="3" customWidth="1"/>
     <col min="5" max="5" width="46" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.34765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1484375" style="1" customWidth="1"/>
     <col min="8" max="8" width="17" style="3" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.34765625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1484375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.34765625" style="1" customWidth="1"/>
     <col min="12" max="12" width="26" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1484375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.34765625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.1484375" style="1" customWidth="1"/>
     <col min="16" max="16" width="12" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6484375" style="1" customWidth="1"/>
     <col min="18" max="18" width="11.5" style="1" customWidth="1"/>
     <col min="19" max="19" width="15" style="1" customWidth="1"/>
     <col min="20" max="21" width="48" style="1" customWidth="1"/>
-    <col min="22" max="22" width="10.83203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="10.84765625" style="1" customWidth="1"/>
     <col min="23" max="23" width="17" style="1" customWidth="1"/>
     <col min="24" max="1025" width="11" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" s="9" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5576,7 +5575,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -5589,7 +5588,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="18.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -5600,7 +5599,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -5613,7 +5612,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -5626,7 +5625,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -5639,7 +5638,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -5652,7 +5651,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27">
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
@@ -5665,7 +5664,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -5681,7 +5680,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27">
       <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
@@ -5694,11 +5693,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27">
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27">
       <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
@@ -5709,13 +5708,13 @@
         <v>376</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -5729,7 +5728,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
@@ -5747,7 +5746,7 @@
       </c>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:27" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27">
       <c r="A15" s="1" t="s">
         <v>111</v>
       </c>
@@ -5758,14 +5757,14 @@
         <v>375</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>378</v>
       </c>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
@@ -5773,7 +5772,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="46.8">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -6302,16 +6301,16 @@
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="15.5" style="10" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="10" customWidth="1"/>
-    <col min="3" max="3" width="39.6640625" style="10" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="10"/>
-    <col min="6" max="1025" width="10.83203125" style="4"/>
+    <col min="3" max="3" width="39.6484375" style="10" customWidth="1"/>
+    <col min="4" max="5" width="10.84765625" style="10"/>
+    <col min="6" max="1025" width="10.84765625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>49</v>
       </c>
@@ -6328,7 +6327,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="10" t="s">
         <v>53</v>
       </c>
@@ -6339,7 +6338,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="10" t="s">
         <v>53</v>
       </c>
@@ -6365,21 +6364,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1484375" customWidth="1"/>
+    <col min="3" max="3" width="13.34765625" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="33" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.6484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="9" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>58</v>
       </c>
@@ -6400,16 +6399,16 @@
       </c>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>383</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>384</v>
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2003261853</v>
+        <v>2003271705</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
@@ -6431,30 +6430,30 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="2" width="36" customWidth="1"/>
     <col min="3" max="3" width="36" style="17" customWidth="1"/>
     <col min="4" max="30" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="15" customHeight="1">
       <c r="A1" s="42" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="42"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" s="43"/>
       <c r="B2" s="43"/>
     </row>
-    <row r="3" spans="1:30" ht="97" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="97" customHeight="1">
       <c r="A3" s="44" t="s">
         <v>66</v>
       </c>
       <c r="B3" s="44"/>
     </row>
-    <row r="5" spans="1:30" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" s="9" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -6546,7 +6545,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="19" customFormat="1" ht="221" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" s="19" customFormat="1" ht="187.2">
       <c r="A6" s="18" t="s">
         <v>74</v>
       </c>
@@ -6638,7 +6637,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" s="22" customFormat="1">
       <c r="A8" s="45" t="s">
         <v>104</v>
       </c>
@@ -6672,7 +6671,7 @@
       <c r="AC8" s="21"/>
       <c r="AD8" s="21"/>
     </row>
-    <row r="10" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" s="25" customFormat="1">
       <c r="A10" s="23" t="s">
         <v>105</v>
       </c>
@@ -6710,7 +6709,7 @@
       <c r="AC10" s="23"/>
       <c r="AD10" s="23"/>
     </row>
-    <row r="11" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" s="25" customFormat="1">
       <c r="A11" s="23" t="s">
         <v>105</v>
       </c>
@@ -6750,7 +6749,7 @@
       <c r="AC11" s="23"/>
       <c r="AD11" s="23"/>
     </row>
-    <row r="12" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" s="25" customFormat="1">
       <c r="A12" s="23" t="s">
         <v>43</v>
       </c>
@@ -6788,7 +6787,7 @@
       <c r="AC12" s="23"/>
       <c r="AD12" s="23"/>
     </row>
-    <row r="13" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" s="25" customFormat="1">
       <c r="A13" s="23" t="s">
         <v>111</v>
       </c>
@@ -6826,7 +6825,7 @@
       <c r="AC13" s="23"/>
       <c r="AD13" s="23"/>
     </row>
-    <row r="14" spans="1:30" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A14" s="23" t="s">
         <v>113</v>
       </c>
@@ -6864,7 +6863,7 @@
       <c r="AC14" s="23"/>
       <c r="AD14" s="23"/>
     </row>
-    <row r="15" spans="1:30" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A15" s="23" t="s">
         <v>113</v>
       </c>
@@ -6904,7 +6903,7 @@
       <c r="AC15" s="23"/>
       <c r="AD15" s="23"/>
     </row>
-    <row r="16" spans="1:30" s="25" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A16" s="23" t="s">
         <v>113</v>
       </c>
@@ -6944,7 +6943,7 @@
       <c r="AC16" s="23"/>
       <c r="AD16" s="23"/>
     </row>
-    <row r="17" spans="1:30" s="25" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A17" s="23" t="s">
         <v>113</v>
       </c>
@@ -6984,7 +6983,7 @@
       <c r="AC17" s="23"/>
       <c r="AD17" s="23"/>
     </row>
-    <row r="18" spans="1:30" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A18" s="23" t="s">
         <v>113</v>
       </c>
@@ -7024,7 +7023,7 @@
       <c r="AC18" s="23"/>
       <c r="AD18" s="23"/>
     </row>
-    <row r="19" spans="1:30" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A19" s="23" t="s">
         <v>113</v>
       </c>
@@ -7064,7 +7063,7 @@
       <c r="AC19" s="23"/>
       <c r="AD19" s="23"/>
     </row>
-    <row r="20" spans="1:30" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A20" s="23" t="s">
         <v>113</v>
       </c>
@@ -7104,7 +7103,7 @@
       <c r="AC20" s="23"/>
       <c r="AD20" s="23"/>
     </row>
-    <row r="21" spans="1:30" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A21" s="23" t="s">
         <v>113</v>
       </c>
@@ -7144,7 +7143,7 @@
       <c r="AC21" s="23"/>
       <c r="AD21" s="23"/>
     </row>
-    <row r="22" spans="1:30" s="25" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A22" s="23" t="s">
         <v>113</v>
       </c>
@@ -7184,7 +7183,7 @@
       <c r="AC22" s="23"/>
       <c r="AD22" s="23"/>
     </row>
-    <row r="23" spans="1:30" s="25" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" s="25" customFormat="1" ht="78">
       <c r="A23" s="23" t="s">
         <v>113</v>
       </c>
@@ -7224,7 +7223,7 @@
       <c r="AC23" s="23"/>
       <c r="AD23" s="23"/>
     </row>
-    <row r="24" spans="1:30" s="25" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A24" s="23" t="s">
         <v>113</v>
       </c>
@@ -7264,7 +7263,7 @@
       <c r="AC24" s="23"/>
       <c r="AD24" s="23"/>
     </row>
-    <row r="25" spans="1:30" s="25" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A25" s="23" t="s">
         <v>113</v>
       </c>
@@ -7304,7 +7303,7 @@
       <c r="AC25" s="23"/>
       <c r="AD25" s="23"/>
     </row>
-    <row r="26" spans="1:30" s="25" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A26" s="23" t="s">
         <v>113</v>
       </c>
@@ -7344,7 +7343,7 @@
       <c r="AC26" s="23"/>
       <c r="AD26" s="23"/>
     </row>
-    <row r="27" spans="1:30" s="25" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A27" s="23" t="s">
         <v>113</v>
       </c>
@@ -7384,7 +7383,7 @@
       <c r="AC27" s="23"/>
       <c r="AD27" s="23"/>
     </row>
-    <row r="28" spans="1:30" s="25" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" s="25" customFormat="1" ht="78">
       <c r="A28" s="23" t="s">
         <v>113</v>
       </c>
@@ -7424,7 +7423,7 @@
       <c r="AC28" s="23"/>
       <c r="AD28" s="23"/>
     </row>
-    <row r="29" spans="1:30" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A29" s="23" t="s">
         <v>143</v>
       </c>
@@ -7462,7 +7461,7 @@
       <c r="AC29" s="23"/>
       <c r="AD29" s="23"/>
     </row>
-    <row r="30" spans="1:30" s="25" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A30" s="23" t="s">
         <v>143</v>
       </c>
@@ -7502,7 +7501,7 @@
       <c r="AC30" s="23"/>
       <c r="AD30" s="23"/>
     </row>
-    <row r="31" spans="1:30" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A31" s="23" t="s">
         <v>143</v>
       </c>
@@ -7542,7 +7541,7 @@
       <c r="AC31" s="23"/>
       <c r="AD31" s="23"/>
     </row>
-    <row r="32" spans="1:30" s="25" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" s="25" customFormat="1" ht="46.8">
       <c r="A32" s="23" t="s">
         <v>143</v>
       </c>
@@ -7582,7 +7581,7 @@
       <c r="AC32" s="23"/>
       <c r="AD32" s="23"/>
     </row>
-    <row r="33" spans="1:30" s="25" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A33" s="23" t="s">
         <v>143</v>
       </c>
@@ -7622,7 +7621,7 @@
       <c r="AC33" s="23"/>
       <c r="AD33" s="23"/>
     </row>
-    <row r="34" spans="1:30" s="25" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A34" s="23" t="s">
         <v>143</v>
       </c>
@@ -7662,7 +7661,7 @@
       <c r="AC34" s="23"/>
       <c r="AD34" s="23"/>
     </row>
-    <row r="35" spans="1:30" s="25" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A35" s="23" t="s">
         <v>143</v>
       </c>
@@ -7702,7 +7701,7 @@
       <c r="AC35" s="23"/>
       <c r="AD35" s="23"/>
     </row>
-    <row r="36" spans="1:30" s="25" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" s="25" customFormat="1" ht="62.4">
       <c r="A36" s="23" t="s">
         <v>143</v>
       </c>
@@ -7742,7 +7741,7 @@
       <c r="AC36" s="23"/>
       <c r="AD36" s="23"/>
     </row>
-    <row r="37" spans="1:30" s="25" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" s="25" customFormat="1" ht="78">
       <c r="A37" s="23" t="s">
         <v>143</v>
       </c>
@@ -7782,7 +7781,7 @@
       <c r="AC37" s="23"/>
       <c r="AD37" s="23"/>
     </row>
-    <row r="38" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:30" s="25" customFormat="1">
       <c r="A38" s="23" t="s">
         <v>153</v>
       </c>
@@ -7820,7 +7819,7 @@
       <c r="AC38" s="23"/>
       <c r="AD38" s="23"/>
     </row>
-    <row r="39" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:30" s="25" customFormat="1">
       <c r="A39" s="23" t="s">
         <v>155</v>
       </c>
@@ -7858,7 +7857,7 @@
       <c r="AC39" s="23"/>
       <c r="AD39" s="23"/>
     </row>
-    <row r="40" spans="1:30" s="25" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A40" s="23" t="s">
         <v>157</v>
       </c>
@@ -7896,7 +7895,7 @@
       <c r="AC40" s="23"/>
       <c r="AD40" s="23"/>
     </row>
-    <row r="41" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" s="25" customFormat="1">
       <c r="A41" s="23" t="s">
         <v>159</v>
       </c>
@@ -7934,7 +7933,7 @@
       <c r="AC41" s="23"/>
       <c r="AD41" s="23"/>
     </row>
-    <row r="42" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:30" s="25" customFormat="1">
       <c r="A42" s="23" t="s">
         <v>161</v>
       </c>
@@ -7972,7 +7971,7 @@
       <c r="AC42" s="23"/>
       <c r="AD42" s="23"/>
     </row>
-    <row r="43" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" s="25" customFormat="1">
       <c r="A43" s="23" t="s">
         <v>161</v>
       </c>
@@ -8012,7 +8011,7 @@
       <c r="AC43" s="23"/>
       <c r="AD43" s="23"/>
     </row>
-    <row r="44" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" s="25" customFormat="1">
       <c r="A44" s="23" t="s">
         <v>165</v>
       </c>
@@ -8050,7 +8049,7 @@
       <c r="AC44" s="23"/>
       <c r="AD44" s="23"/>
     </row>
-    <row r="45" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" s="25" customFormat="1">
       <c r="A45" s="23" t="s">
         <v>165</v>
       </c>
@@ -8090,7 +8089,7 @@
       <c r="AC45" s="23"/>
       <c r="AD45" s="23"/>
     </row>
-    <row r="46" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" s="25" customFormat="1">
       <c r="A46" s="23" t="s">
         <v>51</v>
       </c>
@@ -8128,7 +8127,7 @@
       <c r="AC46" s="23"/>
       <c r="AD46" s="23"/>
     </row>
-    <row r="47" spans="1:30" s="25" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A47" s="23" t="s">
         <v>51</v>
       </c>
@@ -8168,7 +8167,7 @@
       <c r="AC47" s="23"/>
       <c r="AD47" s="23"/>
     </row>
-    <row r="48" spans="1:30" s="25" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A48" s="23" t="s">
         <v>51</v>
       </c>
@@ -8208,7 +8207,7 @@
       <c r="AC48" s="23"/>
       <c r="AD48" s="23"/>
     </row>
-    <row r="49" spans="1:30" s="25" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A49" s="23" t="s">
         <v>51</v>
       </c>
@@ -8248,7 +8247,7 @@
       <c r="AC49" s="23"/>
       <c r="AD49" s="23"/>
     </row>
-    <row r="50" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:30" s="25" customFormat="1">
       <c r="A50" s="23" t="s">
         <v>175</v>
       </c>
@@ -8286,7 +8285,7 @@
       <c r="AC50" s="23"/>
       <c r="AD50" s="23"/>
     </row>
-    <row r="51" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:30" s="25" customFormat="1">
       <c r="A51" s="23" t="s">
         <v>177</v>
       </c>
@@ -8324,7 +8323,7 @@
       <c r="AC51" s="23"/>
       <c r="AD51" s="23"/>
     </row>
-    <row r="52" spans="1:30" s="25" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:30" s="25" customFormat="1" ht="31.2">
       <c r="A52" s="23" t="s">
         <v>179</v>
       </c>
@@ -8362,7 +8361,7 @@
       <c r="AC52" s="23"/>
       <c r="AD52" s="23"/>
     </row>
-    <row r="53" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:30" s="25" customFormat="1">
       <c r="A53" s="23" t="s">
         <v>23</v>
       </c>
@@ -8400,7 +8399,7 @@
       <c r="AC53" s="23"/>
       <c r="AD53" s="23"/>
     </row>
-    <row r="54" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:30" s="25" customFormat="1">
       <c r="A54" s="23" t="s">
         <v>27</v>
       </c>
@@ -8436,7 +8435,7 @@
       <c r="AC54" s="23"/>
       <c r="AD54" s="23"/>
     </row>
-    <row r="55" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:30" s="25" customFormat="1">
       <c r="A55" s="23" t="s">
         <v>30</v>
       </c>
@@ -8472,7 +8471,7 @@
       <c r="AC55" s="23"/>
       <c r="AD55" s="23"/>
     </row>
-    <row r="56" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:30" s="25" customFormat="1">
       <c r="A56" s="23" t="s">
         <v>32</v>
       </c>
@@ -8508,7 +8507,7 @@
       <c r="AC56" s="23"/>
       <c r="AD56" s="23"/>
     </row>
-    <row r="57" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:30" s="25" customFormat="1">
       <c r="A57" s="23" t="s">
         <v>33</v>
       </c>
@@ -8544,7 +8543,7 @@
       <c r="AC57" s="23"/>
       <c r="AD57" s="23"/>
     </row>
-    <row r="58" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:30" s="25" customFormat="1">
       <c r="A58" s="23" t="s">
         <v>34</v>
       </c>
@@ -8580,7 +8579,7 @@
       <c r="AC58" s="23"/>
       <c r="AD58" s="23"/>
     </row>
-    <row r="59" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:30" s="25" customFormat="1">
       <c r="A59" s="23" t="s">
         <v>42</v>
       </c>
@@ -8616,7 +8615,7 @@
       <c r="AC59" s="23"/>
       <c r="AD59" s="23"/>
     </row>
-    <row r="60" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:30" s="25" customFormat="1">
       <c r="A60" s="23" t="s">
         <v>36</v>
       </c>
@@ -8652,7 +8651,7 @@
       <c r="AC60" s="23"/>
       <c r="AD60" s="23"/>
     </row>
-    <row r="61" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:30" s="25" customFormat="1">
       <c r="A61" s="23" t="s">
         <v>182</v>
       </c>
@@ -8688,7 +8687,7 @@
       <c r="AC61" s="23"/>
       <c r="AD61" s="23"/>
     </row>
-    <row r="62" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:30" s="25" customFormat="1">
       <c r="A62" s="23" t="s">
         <v>39</v>
       </c>
@@ -8726,7 +8725,7 @@
       <c r="AC62" s="23"/>
       <c r="AD62" s="23"/>
     </row>
-    <row r="63" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:30" s="25" customFormat="1">
       <c r="A63" s="23" t="s">
         <v>184</v>
       </c>
@@ -8764,7 +8763,7 @@
       <c r="AC63" s="23"/>
       <c r="AD63" s="23"/>
     </row>
-    <row r="64" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:30" s="25" customFormat="1">
       <c r="A64" s="23" t="s">
         <v>186</v>
       </c>
@@ -8802,7 +8801,7 @@
       <c r="AC64" s="23"/>
       <c r="AD64" s="23"/>
     </row>
-    <row r="65" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:30" s="25" customFormat="1">
       <c r="A65" s="23" t="s">
         <v>188</v>
       </c>
@@ -8840,7 +8839,7 @@
       <c r="AC65" s="23"/>
       <c r="AD65" s="23"/>
     </row>
-    <row r="66" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:30" s="25" customFormat="1">
       <c r="A66" s="23" t="s">
         <v>188</v>
       </c>
@@ -8878,7 +8877,7 @@
       <c r="AC66" s="23"/>
       <c r="AD66" s="23"/>
     </row>
-    <row r="67" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:30" s="25" customFormat="1">
       <c r="A67" s="23" t="s">
         <v>188</v>
       </c>
@@ -8916,7 +8915,7 @@
       <c r="AC67" s="23"/>
       <c r="AD67" s="23"/>
     </row>
-    <row r="68" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:30" s="25" customFormat="1">
       <c r="A68" s="23" t="s">
         <v>44</v>
       </c>
@@ -8954,7 +8953,7 @@
       <c r="AC68" s="23"/>
       <c r="AD68" s="23"/>
     </row>
-    <row r="69" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:30" s="25" customFormat="1">
       <c r="A69" s="23" t="s">
         <v>194</v>
       </c>
@@ -8988,7 +8987,7 @@
       <c r="AC69" s="23"/>
       <c r="AD69" s="23"/>
     </row>
-    <row r="70" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:30" s="25" customFormat="1">
       <c r="A70" s="23" t="s">
         <v>48</v>
       </c>
@@ -9024,7 +9023,7 @@
       <c r="AC70" s="23"/>
       <c r="AD70" s="23"/>
     </row>
-    <row r="71" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:30" s="25" customFormat="1">
       <c r="A71" s="23" t="s">
         <v>195</v>
       </c>
@@ -9062,7 +9061,7 @@
       <c r="AC71" s="23"/>
       <c r="AD71" s="23"/>
     </row>
-    <row r="72" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:30" s="25" customFormat="1">
       <c r="A72" s="23" t="s">
         <v>194</v>
       </c>
@@ -9096,7 +9095,7 @@
       <c r="AC72" s="23"/>
       <c r="AD72" s="23"/>
     </row>
-    <row r="73" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:30" s="25" customFormat="1">
       <c r="A73" s="23" t="s">
         <v>198</v>
       </c>
@@ -9132,7 +9131,7 @@
       <c r="AC73" s="23"/>
       <c r="AD73" s="23"/>
     </row>
-    <row r="74" spans="1:30" s="25" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:30" s="25" customFormat="1">
       <c r="A74" s="23" t="s">
         <v>195</v>
       </c>
@@ -9172,7 +9171,7 @@
       <c r="AC74" s="23"/>
       <c r="AD74" s="23"/>
     </row>
-    <row r="75" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:30" s="25" customFormat="1">
       <c r="A75" s="23" t="s">
         <v>194</v>
       </c>
@@ -9206,7 +9205,7 @@
       <c r="AC75" s="23"/>
       <c r="AD75" s="23"/>
     </row>
-    <row r="76" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:30" s="25" customFormat="1">
       <c r="A76" s="23" t="s">
         <v>198</v>
       </c>
@@ -9242,7 +9241,7 @@
       <c r="AC76" s="23"/>
       <c r="AD76" s="23"/>
     </row>
-    <row r="77" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:30" s="25" customFormat="1">
       <c r="A77" s="23" t="s">
         <v>200</v>
       </c>
@@ -9278,7 +9277,7 @@
       <c r="AC77" s="23"/>
       <c r="AD77" s="23"/>
     </row>
-    <row r="78" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:30" s="25" customFormat="1">
       <c r="A78" s="23" t="s">
         <v>201</v>
       </c>
@@ -9314,7 +9313,7 @@
       <c r="AC78" s="23"/>
       <c r="AD78" s="23"/>
     </row>
-    <row r="79" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:30" s="25" customFormat="1">
       <c r="A79" s="23" t="s">
         <v>202</v>
       </c>
@@ -9352,7 +9351,7 @@
       <c r="AC79" s="23"/>
       <c r="AD79" s="23"/>
     </row>
-    <row r="80" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:30" s="25" customFormat="1">
       <c r="A80" s="23" t="s">
         <v>204</v>
       </c>
@@ -9390,7 +9389,7 @@
       <c r="AC80" s="23"/>
       <c r="AD80" s="23"/>
     </row>
-    <row r="81" spans="1:30" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:30" s="25" customFormat="1">
       <c r="A81" s="23" t="s">
         <v>206</v>
       </c>
@@ -9428,7 +9427,7 @@
       <c r="AC81" s="23"/>
       <c r="AD81" s="23"/>
     </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:30">
       <c r="A83" s="46" t="s">
         <v>208</v>
       </c>
@@ -9462,7 +9461,7 @@
       <c r="AC83" s="30"/>
       <c r="AD83" s="30"/>
     </row>
-    <row r="85" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:30">
       <c r="A85" s="31" t="s">
         <v>209</v>
       </c>
@@ -9476,7 +9475,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="86" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:30">
       <c r="A86" s="32" t="s">
         <v>213</v>
       </c>
@@ -9490,7 +9489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:30">
       <c r="A87" s="32" t="s">
         <v>216</v>
       </c>
@@ -9505,7 +9504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:30">
       <c r="A88" s="32" t="s">
         <v>218</v>
       </c>
@@ -9519,7 +9518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:30">
       <c r="A89" s="32" t="s">
         <v>221</v>
       </c>
@@ -9533,7 +9532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:30">
       <c r="A90" s="32" t="s">
         <v>224</v>
       </c>
@@ -9547,7 +9546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:30">
       <c r="A91" s="32" t="s">
         <v>227</v>
       </c>
@@ -9561,7 +9560,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:30">
       <c r="A92" s="32" t="s">
         <v>231</v>
       </c>
@@ -9575,7 +9574,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="93" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:30">
       <c r="A93" s="32" t="s">
         <v>234</v>
       </c>
@@ -9589,7 +9588,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="94" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:30">
       <c r="A94" s="32" t="s">
         <v>237</v>
       </c>
@@ -9603,7 +9602,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="95" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:30">
       <c r="A95" s="32" t="s">
         <v>240</v>
       </c>
@@ -9617,7 +9616,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="96" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:30">
       <c r="A96" s="32" t="s">
         <v>243</v>
       </c>
@@ -9631,7 +9630,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4">
       <c r="A97" s="32" t="s">
         <v>246</v>
       </c>
@@ -9645,7 +9644,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4">
       <c r="A98" s="32" t="s">
         <v>249</v>
       </c>
@@ -9659,7 +9658,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4">
       <c r="A99" s="32" t="s">
         <v>252</v>
       </c>
@@ -9673,13 +9672,13 @@
         <v>255</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4">
       <c r="A100" s="29"/>
       <c r="B100" s="29"/>
       <c r="C100" s="28"/>
       <c r="D100" s="29"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4">
       <c r="A101" s="29"/>
       <c r="B101" s="31" t="s">
         <v>256</v>
@@ -9689,7 +9688,7 @@
       </c>
       <c r="D101" s="29"/>
     </row>
-    <row r="102" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4">
       <c r="A102" s="29"/>
       <c r="B102" s="34" t="s">
         <v>257</v>
@@ -9699,7 +9698,7 @@
       </c>
       <c r="D102" s="29"/>
     </row>
-    <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4">
       <c r="A103" s="29"/>
       <c r="B103" s="35" t="s">
         <v>258</v>
@@ -9709,7 +9708,7 @@
       </c>
       <c r="D103" s="29"/>
     </row>
-    <row r="104" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" ht="31.2">
       <c r="A104" s="29"/>
       <c r="B104" s="35" t="s">
         <v>259</v>
@@ -9719,7 +9718,7 @@
       </c>
       <c r="D104" s="29"/>
     </row>
-    <row r="105" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4">
       <c r="A105" s="29"/>
       <c r="B105" s="35" t="s">
         <v>261</v>
@@ -9729,7 +9728,7 @@
       </c>
       <c r="D105" s="29"/>
     </row>
-    <row r="106" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4">
       <c r="A106" s="29"/>
       <c r="B106" s="35" t="s">
         <v>263</v>
@@ -9739,7 +9738,7 @@
       </c>
       <c r="D106" s="29"/>
     </row>
-    <row r="107" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4">
       <c r="A107" s="29"/>
       <c r="B107" s="35" t="s">
         <v>265</v>
@@ -9749,7 +9748,7 @@
       </c>
       <c r="D107" s="29"/>
     </row>
-    <row r="108" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4">
       <c r="A108" s="29"/>
       <c r="B108" s="35" t="s">
         <v>267</v>
@@ -9759,7 +9758,7 @@
       </c>
       <c r="D108" s="29"/>
     </row>
-    <row r="109" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" ht="46.8">
       <c r="A109" s="29"/>
       <c r="B109" s="35" t="s">
         <v>269</v>
@@ -9769,7 +9768,7 @@
       </c>
       <c r="D109" s="29"/>
     </row>
-    <row r="110" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4">
       <c r="A110" s="29"/>
       <c r="B110" s="35" t="s">
         <v>271</v>
@@ -9779,7 +9778,7 @@
       </c>
       <c r="D110" s="29"/>
     </row>
-    <row r="111" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4">
       <c r="A111" s="29"/>
       <c r="B111" s="35" t="s">
         <v>273</v>
@@ -9789,7 +9788,7 @@
       </c>
       <c r="D111" s="29"/>
     </row>
-    <row r="112" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4">
       <c r="A112" s="29"/>
       <c r="B112" s="35" t="s">
         <v>274</v>
@@ -9799,7 +9798,7 @@
       </c>
       <c r="D112" s="29"/>
     </row>
-    <row r="113" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4">
       <c r="A113" s="29"/>
       <c r="B113" s="35" t="s">
         <v>276</v>
@@ -9809,7 +9808,7 @@
       </c>
       <c r="D113" s="29"/>
     </row>
-    <row r="114" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4">
       <c r="A114" s="29"/>
       <c r="B114" s="35" t="s">
         <v>278</v>
@@ -9819,7 +9818,7 @@
       </c>
       <c r="D114" s="29"/>
     </row>
-    <row r="115" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4">
       <c r="A115" s="29"/>
       <c r="B115" s="35" t="s">
         <v>280</v>
@@ -9829,7 +9828,7 @@
       </c>
       <c r="D115" s="29"/>
     </row>
-    <row r="116" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4">
       <c r="A116" s="29"/>
       <c r="B116" s="35" t="s">
         <v>282</v>
@@ -9839,7 +9838,7 @@
       </c>
       <c r="D116" s="29"/>
     </row>
-    <row r="117" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="31.2">
       <c r="A117" s="29"/>
       <c r="B117" s="35" t="s">
         <v>284</v>
@@ -9849,7 +9848,7 @@
       </c>
       <c r="D117" s="29"/>
     </row>
-    <row r="118" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4">
       <c r="A118" s="29"/>
       <c r="B118" s="35" t="s">
         <v>286</v>
@@ -9859,7 +9858,7 @@
       </c>
       <c r="D118" s="29"/>
     </row>
-    <row r="119" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4">
       <c r="A119" s="29"/>
       <c r="B119" s="35" t="s">
         <v>288</v>
@@ -9869,7 +9868,7 @@
       </c>
       <c r="D119" s="29"/>
     </row>
-    <row r="120" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4">
       <c r="A120" s="29"/>
       <c r="B120" s="35" t="s">
         <v>290</v>
@@ -9879,7 +9878,7 @@
       </c>
       <c r="D120" s="29"/>
     </row>
-    <row r="121" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" ht="31.2">
       <c r="A121" s="29"/>
       <c r="B121" s="35" t="s">
         <v>292</v>
@@ -9889,7 +9888,7 @@
       </c>
       <c r="D121" s="29"/>
     </row>
-    <row r="122" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="46.8">
       <c r="A122" s="29"/>
       <c r="B122" s="35" t="s">
         <v>294</v>
@@ -9899,7 +9898,7 @@
       </c>
       <c r="D122" s="29"/>
     </row>
-    <row r="123" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4">
       <c r="A123" s="29"/>
       <c r="B123" s="35" t="s">
         <v>296</v>
@@ -9909,7 +9908,7 @@
       </c>
       <c r="D123" s="29"/>
     </row>
-    <row r="124" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4">
       <c r="A124" s="29"/>
       <c r="B124" s="35" t="s">
         <v>298</v>
@@ -9919,7 +9918,7 @@
       </c>
       <c r="D124" s="29"/>
     </row>
-    <row r="125" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4">
       <c r="A125" s="29"/>
       <c r="B125" s="35" t="s">
         <v>300</v>
@@ -9929,7 +9928,7 @@
       </c>
       <c r="D125" s="29"/>
     </row>
-    <row r="126" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4">
       <c r="A126" s="29"/>
       <c r="B126" s="35" t="s">
         <v>302</v>
@@ -9939,7 +9938,7 @@
       </c>
       <c r="D126" s="29"/>
     </row>
-    <row r="127" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4">
       <c r="A127" s="29"/>
       <c r="B127" s="35" t="s">
         <v>304</v>
@@ -9949,7 +9948,7 @@
       </c>
       <c r="D127" s="29"/>
     </row>
-    <row r="128" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" ht="31.2">
       <c r="A128" s="29"/>
       <c r="B128" s="35" t="s">
         <v>306</v>
@@ -9959,7 +9958,7 @@
       </c>
       <c r="D128" s="29"/>
     </row>
-    <row r="129" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4">
       <c r="A129" s="29"/>
       <c r="B129" s="36" t="s">
         <v>308</v>
@@ -9969,7 +9968,7 @@
       </c>
       <c r="D129" s="29"/>
     </row>
-    <row r="130" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" ht="31.2">
       <c r="A130" s="29"/>
       <c r="B130" s="36" t="s">
         <v>310</v>
@@ -9979,7 +9978,7 @@
       </c>
       <c r="D130" s="29"/>
     </row>
-    <row r="131" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4">
       <c r="A131" s="29"/>
       <c r="B131" s="36" t="s">
         <v>311</v>
@@ -9989,7 +9988,7 @@
       </c>
       <c r="D131" s="29"/>
     </row>
-    <row r="132" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4">
       <c r="A132" s="29"/>
       <c r="B132" s="36" t="s">
         <v>312</v>
@@ -9999,7 +9998,7 @@
       </c>
       <c r="D132" s="29"/>
     </row>
-    <row r="133" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4">
       <c r="A133" s="29"/>
       <c r="B133" s="36" t="s">
         <v>313</v>
@@ -10009,7 +10008,7 @@
       </c>
       <c r="D133" s="29"/>
     </row>
-    <row r="134" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4">
       <c r="A134" s="29"/>
       <c r="B134" s="36" t="s">
         <v>41</v>
@@ -10019,7 +10018,7 @@
       </c>
       <c r="D134" s="29"/>
     </row>
-    <row r="135" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4">
       <c r="A135" s="29"/>
       <c r="B135" s="36" t="s">
         <v>314</v>
@@ -10029,7 +10028,7 @@
       </c>
       <c r="D135" s="29"/>
     </row>
-    <row r="136" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4">
       <c r="A136" s="29"/>
       <c r="B136" s="36" t="s">
         <v>316</v>
@@ -10039,7 +10038,7 @@
       </c>
       <c r="D136" s="29"/>
     </row>
-    <row r="137" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4">
       <c r="A137" s="29"/>
       <c r="B137" s="36" t="s">
         <v>317</v>
@@ -10049,7 +10048,7 @@
       </c>
       <c r="D137" s="29"/>
     </row>
-    <row r="138" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" ht="31.2">
       <c r="A138" s="29"/>
       <c r="B138" s="36" t="s">
         <v>319</v>
@@ -10059,7 +10058,7 @@
       </c>
       <c r="D138" s="29"/>
     </row>
-    <row r="139" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4">
       <c r="A139" s="29"/>
       <c r="B139" s="36" t="s">
         <v>321</v>
@@ -10069,7 +10068,7 @@
       </c>
       <c r="D139" s="29"/>
     </row>
-    <row r="140" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" ht="31.2">
       <c r="A140" s="29"/>
       <c r="B140" s="36" t="s">
         <v>323</v>
@@ -10079,7 +10078,7 @@
       </c>
       <c r="D140" s="29"/>
     </row>
-    <row r="141" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4">
       <c r="A141" s="29"/>
       <c r="B141" s="36" t="s">
         <v>325</v>
@@ -10089,7 +10088,7 @@
       </c>
       <c r="D141" s="29"/>
     </row>
-    <row r="142" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4">
       <c r="A142" s="29"/>
       <c r="B142" s="36" t="s">
         <v>327</v>
@@ -10099,7 +10098,7 @@
       </c>
       <c r="D142" s="29"/>
     </row>
-    <row r="143" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" ht="31.2">
       <c r="A143" s="29"/>
       <c r="B143" s="36" t="s">
         <v>329</v>
@@ -10109,7 +10108,7 @@
       </c>
       <c r="D143" s="29"/>
     </row>
-    <row r="144" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4">
       <c r="A144" s="29"/>
       <c r="B144" s="36" t="s">
         <v>331</v>
@@ -10119,7 +10118,7 @@
       </c>
       <c r="D144" s="29"/>
     </row>
-    <row r="145" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4">
       <c r="A145" s="29"/>
       <c r="B145" s="36" t="s">
         <v>333</v>
@@ -10129,7 +10128,7 @@
       </c>
       <c r="D145" s="29"/>
     </row>
-    <row r="146" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4">
       <c r="A146" s="29"/>
       <c r="B146" s="36" t="s">
         <v>335</v>
@@ -10139,7 +10138,7 @@
       </c>
       <c r="D146" s="29"/>
     </row>
-    <row r="147" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4">
       <c r="A147" s="29"/>
       <c r="B147" s="36" t="s">
         <v>337</v>
@@ -10149,7 +10148,7 @@
       </c>
       <c r="D147" s="29"/>
     </row>
-    <row r="148" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4">
       <c r="A148" s="29"/>
       <c r="B148" s="36" t="s">
         <v>339</v>
@@ -10159,7 +10158,7 @@
       </c>
       <c r="D148" s="29"/>
     </row>
-    <row r="149" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4">
       <c r="A149" s="29"/>
       <c r="B149" s="36" t="s">
         <v>341</v>
@@ -10169,7 +10168,7 @@
       </c>
       <c r="D149" s="29"/>
     </row>
-    <row r="150" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4">
       <c r="A150" s="29"/>
       <c r="B150" s="36" t="s">
         <v>343</v>
@@ -10179,7 +10178,7 @@
       </c>
       <c r="D150" s="29"/>
     </row>
-    <row r="151" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4">
       <c r="A151" s="29"/>
       <c r="B151" s="36" t="s">
         <v>345</v>
@@ -10189,7 +10188,7 @@
       </c>
       <c r="D151" s="29"/>
     </row>
-    <row r="152" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4">
       <c r="A152" s="29"/>
       <c r="B152" s="36" t="s">
         <v>347</v>
@@ -10199,7 +10198,7 @@
       </c>
       <c r="D152" s="29"/>
     </row>
-    <row r="153" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4">
       <c r="A153" s="29"/>
       <c r="B153" s="36" t="s">
         <v>349</v>
@@ -10209,7 +10208,7 @@
       </c>
       <c r="D153" s="29"/>
     </row>
-    <row r="154" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4">
       <c r="A154" s="29"/>
       <c r="B154" s="36" t="s">
         <v>351</v>
@@ -10586,28 +10585,28 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="7" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="42" t="s">
         <v>352</v>
       </c>
       <c r="B1" s="42"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="43"/>
       <c r="B2" s="43"/>
     </row>
-    <row r="3" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="99" customHeight="1">
       <c r="A3" s="44" t="s">
         <v>353</v>
       </c>
       <c r="B3" s="44"/>
     </row>
-    <row r="5" spans="1:8" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="9" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="11" t="s">
         <v>49</v>
       </c>
@@ -10630,7 +10629,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="19" customFormat="1" ht="221" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" s="19" customFormat="1" ht="202.8">
       <c r="A6" s="18" t="s">
         <v>355</v>
       </c>
@@ -10673,12 +10672,12 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="6" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="16" customHeight="1">
       <c r="A1" s="47" t="s">
         <v>361</v>
       </c>
@@ -10688,7 +10687,7 @@
       <c r="E1" s="38"/>
       <c r="F1" s="38"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="43"/>
       <c r="B2" s="43"/>
       <c r="C2" s="38"/>
@@ -10696,7 +10695,7 @@
       <c r="E2" s="38"/>
       <c r="F2" s="38"/>
     </row>
-    <row r="3" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="55" customHeight="1">
       <c r="A3" s="44" t="s">
         <v>362</v>
       </c>
@@ -10706,7 +10705,7 @@
       <c r="E3" s="38"/>
       <c r="F3" s="38"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="38"/>
       <c r="B4" s="38"/>
       <c r="C4" s="38"/>
@@ -10714,7 +10713,7 @@
       <c r="E4" s="38"/>
       <c r="F4" s="38"/>
     </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="5" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="39" t="s">
         <v>58</v>
       </c>
@@ -10735,7 +10734,7 @@
       </c>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" s="19" customFormat="1" ht="340" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" s="19" customFormat="1" ht="296.39999999999998">
       <c r="A6" s="18" t="s">
         <v>363</v>
       </c>
@@ -10755,7 +10754,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="41"/>
       <c r="B7" s="41"/>
       <c r="C7" s="41"/>
@@ -10763,7 +10762,7 @@
       <c r="E7" s="41"/>
       <c r="F7" s="41"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="41"/>
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>

</xml_diff>